<commit_message>
Update iso code file with manual edits
</commit_message>
<xml_diff>
--- a/Data/iso_codes.xlsx
+++ b/Data/iso_codes.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I254"/>
+  <dimension ref="A1:I256"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -2921,46 +2921,46 @@
     </row>
     <row r="76">
       <c r="A76">
-        <v>46571</v>
+        <v>31799</v>
       </c>
       <c r="B76" t="inlineStr">
         <is>
-          <t>Bonaire</t>
+          <t>Bermuda</t>
         </is>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Bonaire</t>
+          <t>Bermudas</t>
+        </is>
+      </c>
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H76" t="inlineStr">
+        <is>
+          <t>BM</t>
+        </is>
+      </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>BMU</t>
         </is>
       </c>
     </row>
     <row r="77">
       <c r="A77">
-        <v>243</v>
+        <v>46571</v>
       </c>
       <c r="B77" t="inlineStr">
         <is>
-          <t>British Virgin Islands</t>
+          <t>Bonaire</t>
         </is>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>British Virgin Islands</t>
-        </is>
-      </c>
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="H77" t="inlineStr">
-        <is>
-          <t>VG</t>
-        </is>
-      </c>
-      <c r="I77" t="inlineStr">
-        <is>
-          <t>VGB</t>
+          <t>Bonaire</t>
         </is>
       </c>
     </row>
@@ -2970,7 +2970,7 @@
       </c>
       <c r="B78" t="inlineStr">
         <is>
-          <t>Islas Vírgenes Británicas</t>
+          <t>British Virgin Islands</t>
         </is>
       </c>
       <c r="C78" t="inlineStr">
@@ -2996,66 +2996,71 @@
     </row>
     <row r="79">
       <c r="A79">
-        <v>31772</v>
+        <v>243</v>
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Islas Vírgenes Británicas</t>
         </is>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>British Virgin Islands</t>
+        </is>
+      </c>
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H79" t="inlineStr">
         <is>
-          <t>BG</t>
+          <t>VG</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
         <is>
-          <t>BGR</t>
+          <t>VGB</t>
         </is>
       </c>
     </row>
     <row r="80">
       <c r="A80">
-        <v>85583</v>
+        <v>31772</v>
       </c>
       <c r="B80" t="inlineStr">
         <is>
-          <t>CELAC</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>CELAC</t>
+          <t>Bulgaria</t>
+        </is>
+      </c>
+      <c r="H80" t="inlineStr">
+        <is>
+          <t>BG</t>
+        </is>
+      </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>BGR</t>
         </is>
       </c>
     </row>
     <row r="81">
       <c r="A81">
-        <v>43440</v>
+        <v>85583</v>
       </c>
       <c r="B81" t="inlineStr">
         <is>
-          <t>Canada</t>
+          <t>CELAC</t>
         </is>
       </c>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Canada</t>
-        </is>
-      </c>
-      <c r="H81" t="inlineStr">
-        <is>
-          <t>CA</t>
-        </is>
-      </c>
-      <c r="I81" t="inlineStr">
-        <is>
-          <t>CAN</t>
+          <t>CELAC</t>
         </is>
       </c>
     </row>
@@ -3065,7 +3070,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>Canadá</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="C82" t="inlineStr">
@@ -3086,26 +3091,26 @@
     </row>
     <row r="83">
       <c r="A83">
-        <v>43439</v>
+        <v>43440</v>
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>Cape Verde</t>
+          <t>Canadá</t>
         </is>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Cape Verde</t>
+          <t>Canada</t>
         </is>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>CV</t>
+          <t>CA</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
         <is>
-          <t>CPV</t>
+          <t>CAN</t>
         </is>
       </c>
     </row>
@@ -3115,7 +3120,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>Cabo Verde</t>
+          <t>Cape Verde</t>
         </is>
       </c>
       <c r="C84" t="inlineStr">
@@ -3136,26 +3141,26 @@
     </row>
     <row r="85">
       <c r="A85">
-        <v>43403</v>
+        <v>43439</v>
       </c>
       <c r="B85" t="inlineStr">
         <is>
-          <t>Caribbean Netherlands</t>
+          <t>Cabo Verde</t>
         </is>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Caribbean Netherlands</t>
+          <t>Cape Verde</t>
         </is>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>BQ</t>
+          <t>CV</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
         <is>
-          <t>BES</t>
+          <t>CPV</t>
         </is>
       </c>
     </row>
@@ -3165,7 +3170,7 @@
       </c>
       <c r="B86" t="inlineStr">
         <is>
-          <t>Caribe neerlandés</t>
+          <t>Caribbean Netherlands</t>
         </is>
       </c>
       <c r="C86" t="inlineStr">
@@ -3186,31 +3191,26 @@
     </row>
     <row r="87">
       <c r="A87">
-        <v>20442</v>
+        <v>43403</v>
       </c>
       <c r="B87" t="inlineStr">
         <is>
-          <t>Cayman Islands</t>
+          <t>Caribe neerlandés</t>
         </is>
       </c>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Cayman Islands</t>
-        </is>
-      </c>
-      <c r="E87" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Caribbean Netherlands</t>
         </is>
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>KY</t>
+          <t>BQ</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
         <is>
-          <t>CYM</t>
+          <t>BES</t>
         </is>
       </c>
     </row>
@@ -3220,7 +3220,7 @@
       </c>
       <c r="B88" t="inlineStr">
         <is>
-          <t>Islas Caimán</t>
+          <t>Cayman Islands</t>
         </is>
       </c>
       <c r="C88" t="inlineStr">
@@ -3246,16 +3246,31 @@
     </row>
     <row r="89">
       <c r="A89">
-        <v>31808</v>
+        <v>20442</v>
       </c>
       <c r="B89" t="inlineStr">
         <is>
-          <t>Central American Common Market (CACM)</t>
+          <t>Islas Caimán</t>
         </is>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Central American Common Market (CACM)</t>
+          <t>Cayman Islands</t>
+        </is>
+      </c>
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H89" t="inlineStr">
+        <is>
+          <t>KY</t>
+        </is>
+      </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>CYM</t>
         </is>
       </c>
     </row>
@@ -3265,7 +3280,7 @@
       </c>
       <c r="B90" t="inlineStr">
         <is>
-          <t>Mercado Común Centroamericano (MCCA)</t>
+          <t>Central American Common Market (CACM)</t>
         </is>
       </c>
       <c r="C90" t="inlineStr">
@@ -3276,41 +3291,41 @@
     </row>
     <row r="91">
       <c r="A91">
-        <v>43441</v>
+        <v>31808</v>
       </c>
       <c r="B91" t="inlineStr">
         <is>
-          <t>China</t>
+          <t>Mercado Común Centroamericano (MCCA)</t>
         </is>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>China</t>
-        </is>
-      </c>
-      <c r="H91" t="inlineStr">
-        <is>
-          <t>CN</t>
-        </is>
-      </c>
-      <c r="I91" t="inlineStr">
-        <is>
-          <t>CHN</t>
+          <t>Central American Common Market (CACM)</t>
         </is>
       </c>
     </row>
     <row r="92">
       <c r="A92">
-        <v>31809</v>
+        <v>43441</v>
       </c>
       <c r="B92" t="inlineStr">
         <is>
-          <t>Common market of the south (MERCOSUR)</t>
+          <t>China</t>
         </is>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Common market of the south (MERCOSUR)</t>
+          <t>China</t>
+        </is>
+      </c>
+      <c r="H92" t="inlineStr">
+        <is>
+          <t>CN</t>
+        </is>
+      </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>CHN</t>
         </is>
       </c>
     </row>
@@ -3320,7 +3335,7 @@
       </c>
       <c r="B93" t="inlineStr">
         <is>
-          <t>Mercado Común del Sur (MERCOSUR)</t>
+          <t>Common market of the south (MERCOSUR)</t>
         </is>
       </c>
       <c r="C93" t="inlineStr">
@@ -3331,16 +3346,16 @@
     </row>
     <row r="94">
       <c r="A94">
-        <v>46573</v>
+        <v>31809</v>
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Common market of the south (MERCOSUR), Bolivia (Plurinational State of) and Chile</t>
+          <t>Mercado Común del Sur (MERCOSUR)</t>
         </is>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Common market of the south (MERCOSUR), Bolivia (Plurinational State of) and Chile</t>
+          <t>Common market of the south (MERCOSUR)</t>
         </is>
       </c>
     </row>
@@ -3350,7 +3365,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Mercado Común del Sur (MERCOSUR), Bolivia (Estado Plurinacional de) y Chile</t>
+          <t>Common market of the south (MERCOSUR), Bolivia (Plurinational State of) and Chile</t>
         </is>
       </c>
       <c r="C95" t="inlineStr">
@@ -3361,26 +3376,16 @@
     </row>
     <row r="96">
       <c r="A96">
-        <v>43442</v>
+        <v>46573</v>
       </c>
       <c r="B96" t="inlineStr">
         <is>
-          <t>Croatia</t>
+          <t>Mercado Común del Sur (MERCOSUR), Bolivia (Estado Plurinacional de) y Chile</t>
         </is>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Croatia</t>
-        </is>
-      </c>
-      <c r="H96" t="inlineStr">
-        <is>
-          <t>HR</t>
-        </is>
-      </c>
-      <c r="I96" t="inlineStr">
-        <is>
-          <t>HRV</t>
+          <t>Common market of the south (MERCOSUR), Bolivia (Plurinational State of) and Chile</t>
         </is>
       </c>
     </row>
@@ -3390,7 +3395,7 @@
       </c>
       <c r="B97" t="inlineStr">
         <is>
-          <t>Croacia</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="C97" t="inlineStr">
@@ -3411,56 +3416,56 @@
     </row>
     <row r="98">
       <c r="A98">
-        <v>43404</v>
+        <v>43442</v>
       </c>
       <c r="B98" t="inlineStr">
         <is>
-          <t>Curaçao</t>
+          <t>Croacia</t>
         </is>
       </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Curaçao</t>
-        </is>
-      </c>
-      <c r="E98" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Croatia</t>
         </is>
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>CW</t>
+          <t>HR</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
         <is>
-          <t>CUW</t>
+          <t>HRV</t>
         </is>
       </c>
     </row>
     <row r="99">
       <c r="A99">
-        <v>31773</v>
+        <v>43404</v>
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Curaçao</t>
         </is>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Curaçao</t>
+        </is>
+      </c>
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>CY</t>
+          <t>CW</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
         <is>
-          <t>CYP</t>
+          <t>CUW</t>
         </is>
       </c>
     </row>
@@ -3470,7 +3475,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>Chipre</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="C100" t="inlineStr">
@@ -3491,26 +3496,26 @@
     </row>
     <row r="101">
       <c r="A101">
-        <v>31791</v>
+        <v>31773</v>
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Chipre</t>
         </is>
       </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Czech Republic</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="H101" t="inlineStr">
         <is>
-          <t>CZ</t>
+          <t>CY</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
         <is>
-          <t>CZE</t>
+          <t>CYP</t>
         </is>
       </c>
     </row>
@@ -3520,7 +3525,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>República Checa</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="C102" t="inlineStr">
@@ -3541,26 +3546,26 @@
     </row>
     <row r="103">
       <c r="A103">
-        <v>43463</v>
+        <v>31791</v>
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>Democratic Peoples Republic of Korea (North Korea)</t>
+          <t>República Checa</t>
         </is>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Democratic Peoples Republic of Korea (North Korea)</t>
+          <t>Czech Republic</t>
         </is>
       </c>
       <c r="H103" t="inlineStr">
         <is>
-          <t>KP</t>
+          <t>CZ</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
         <is>
-          <t>PRK</t>
+          <t>CZE</t>
         </is>
       </c>
     </row>
@@ -3570,7 +3575,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>República Popular Democrática de Corea (Corea del Norte)</t>
+          <t>Democratic Peoples Republic of Korea (North Korea)</t>
         </is>
       </c>
       <c r="C104" t="inlineStr">
@@ -3591,26 +3596,26 @@
     </row>
     <row r="105">
       <c r="A105">
-        <v>31774</v>
+        <v>43463</v>
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>República Popular Democrática de Corea (Corea del Norte)</t>
         </is>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Denmark</t>
+          <t>Democratic Peoples Republic of Korea (North Korea)</t>
         </is>
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>DK</t>
+          <t>KP</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
         <is>
-          <t>DNK</t>
+          <t>PRK</t>
         </is>
       </c>
     </row>
@@ -3620,7 +3625,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>Dinamarca</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="C106" t="inlineStr">
@@ -3641,26 +3646,26 @@
     </row>
     <row r="107">
       <c r="A107">
-        <v>43444</v>
+        <v>31774</v>
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Dinamarca</t>
         </is>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Denmark</t>
         </is>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>EG</t>
+          <t>DK</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
         <is>
-          <t>EGY</t>
+          <t>DNK</t>
         </is>
       </c>
     </row>
@@ -3670,7 +3675,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>Egipto</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="C108" t="inlineStr">
@@ -3691,16 +3696,26 @@
     </row>
     <row r="109">
       <c r="A109">
-        <v>43468</v>
+        <v>43444</v>
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Egipto</t>
         </is>
       </c>
       <c r="C109" t="inlineStr">
         <is>
-          <t>England</t>
+          <t>Egypt</t>
+        </is>
+      </c>
+      <c r="H109" t="inlineStr">
+        <is>
+          <t>EG</t>
+        </is>
+      </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>EGY</t>
         </is>
       </c>
     </row>
@@ -3710,7 +3725,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>Inglaterra</t>
+          <t>England</t>
         </is>
       </c>
       <c r="C110" t="inlineStr">
@@ -3721,41 +3736,41 @@
     </row>
     <row r="111">
       <c r="A111">
-        <v>31777</v>
+        <v>43468</v>
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>Estonia</t>
+          <t>Inglaterra</t>
         </is>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Estonia</t>
-        </is>
-      </c>
-      <c r="H111" t="inlineStr">
-        <is>
-          <t>EE</t>
-        </is>
-      </c>
-      <c r="I111" t="inlineStr">
-        <is>
-          <t>EST</t>
+          <t>England</t>
         </is>
       </c>
     </row>
     <row r="112">
       <c r="A112">
-        <v>31797</v>
+        <v>31777</v>
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Estonia</t>
         </is>
       </c>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Europe</t>
+          <t>Estonia</t>
+        </is>
+      </c>
+      <c r="H112" t="inlineStr">
+        <is>
+          <t>EE</t>
+        </is>
+      </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>EST</t>
         </is>
       </c>
     </row>
@@ -3765,7 +3780,7 @@
       </c>
       <c r="B113" t="inlineStr">
         <is>
-          <t>Europa</t>
+          <t>Europe</t>
         </is>
       </c>
       <c r="C113" t="inlineStr">
@@ -3776,16 +3791,16 @@
     </row>
     <row r="114">
       <c r="A114">
-        <v>31798</v>
+        <v>31797</v>
       </c>
       <c r="B114" t="inlineStr">
         <is>
-          <t>European Union</t>
+          <t>Europa</t>
         </is>
       </c>
       <c r="C114" t="inlineStr">
         <is>
-          <t>European Union</t>
+          <t>Europe</t>
         </is>
       </c>
     </row>
@@ -3795,7 +3810,7 @@
       </c>
       <c r="B115" t="inlineStr">
         <is>
-          <t>Unión Europea</t>
+          <t>European Union</t>
         </is>
       </c>
       <c r="C115" t="inlineStr">
@@ -3806,16 +3821,16 @@
     </row>
     <row r="116">
       <c r="A116">
-        <v>31794</v>
+        <v>31798</v>
       </c>
       <c r="B116" t="inlineStr">
         <is>
-          <t>European Union (15 countries)</t>
+          <t>Unión Europea</t>
         </is>
       </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>European Union (15 countries)</t>
+          <t>European Union</t>
         </is>
       </c>
     </row>
@@ -3825,7 +3840,7 @@
       </c>
       <c r="B117" t="inlineStr">
         <is>
-          <t>Unión Europea (15 países)</t>
+          <t>European Union (15 countries)</t>
         </is>
       </c>
       <c r="C117" t="inlineStr">
@@ -3836,16 +3851,16 @@
     </row>
     <row r="118">
       <c r="A118">
-        <v>31795</v>
+        <v>31794</v>
       </c>
       <c r="B118" t="inlineStr">
         <is>
-          <t>European Union (25 countries)</t>
+          <t>Unión Europea (15 países)</t>
         </is>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>European Union (25 countries)</t>
+          <t>European Union (15 countries)</t>
         </is>
       </c>
     </row>
@@ -3855,7 +3870,7 @@
       </c>
       <c r="B119" t="inlineStr">
         <is>
-          <t>Unión Europea (25 países)</t>
+          <t>European Union (25 countries)</t>
         </is>
       </c>
       <c r="C119" t="inlineStr">
@@ -3866,16 +3881,16 @@
     </row>
     <row r="120">
       <c r="A120">
-        <v>31796</v>
+        <v>31795</v>
       </c>
       <c r="B120" t="inlineStr">
         <is>
-          <t>European Union (27 countries)</t>
+          <t>Unión Europea (25 países)</t>
         </is>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>European Union (27 countries)</t>
+          <t>European Union (25 countries)</t>
         </is>
       </c>
     </row>
@@ -3885,7 +3900,7 @@
       </c>
       <c r="B121" t="inlineStr">
         <is>
-          <t>Unión Europea (27 países)</t>
+          <t>European Union (27 countries)</t>
         </is>
       </c>
       <c r="C121" t="inlineStr">
@@ -3896,16 +3911,16 @@
     </row>
     <row r="122">
       <c r="A122">
-        <v>43529</v>
+        <v>31796</v>
       </c>
       <c r="B122" t="inlineStr">
         <is>
-          <t>European Union (28 countries)</t>
+          <t>Unión Europea (27 países)</t>
         </is>
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>European Union (28 countries)</t>
+          <t>European Union (27 countries)</t>
         </is>
       </c>
     </row>
@@ -3915,7 +3930,7 @@
       </c>
       <c r="B123" t="inlineStr">
         <is>
-          <t>Unión Europea (28 países)</t>
+          <t>European Union (28 countries)</t>
         </is>
       </c>
       <c r="C123" t="inlineStr">
@@ -3926,26 +3941,16 @@
     </row>
     <row r="124">
       <c r="A124">
-        <v>31801</v>
+        <v>43529</v>
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>Falkland Islands (Malvinas)</t>
+          <t>Unión Europea (28 países)</t>
         </is>
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Falkland Islands (Malvinas)</t>
-        </is>
-      </c>
-      <c r="H124" t="inlineStr">
-        <is>
-          <t>FK</t>
-        </is>
-      </c>
-      <c r="I124" t="inlineStr">
-        <is>
-          <t>FLK</t>
+          <t>European Union (28 countries)</t>
         </is>
       </c>
     </row>
@@ -3955,7 +3960,7 @@
       </c>
       <c r="B125" t="inlineStr">
         <is>
-          <t>Islas Malvinas</t>
+          <t>Falkland Islands (Malvinas)</t>
         </is>
       </c>
       <c r="C125" t="inlineStr">
@@ -3976,26 +3981,26 @@
     </row>
     <row r="126">
       <c r="A126">
-        <v>31778</v>
+        <v>31801</v>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Islas Malvinas</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Finland</t>
+          <t>Falkland Islands (Malvinas)</t>
         </is>
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>FI</t>
+          <t>FK</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
         <is>
-          <t>FIN</t>
+          <t>FLK</t>
         </is>
       </c>
     </row>
@@ -4005,7 +4010,7 @@
       </c>
       <c r="B127" t="inlineStr">
         <is>
-          <t>Finlandia</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="C127" t="inlineStr">
@@ -4026,26 +4031,26 @@
     </row>
     <row r="128">
       <c r="A128">
-        <v>31779</v>
+        <v>31778</v>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Finlandia</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Finland</t>
         </is>
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>FR</t>
+          <t>FI</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
         <is>
-          <t>FRA</t>
+          <t>FIN</t>
         </is>
       </c>
     </row>
@@ -4055,7 +4060,7 @@
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>Francia</t>
+          <t>France</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
@@ -4076,31 +4081,26 @@
     </row>
     <row r="130">
       <c r="A130">
-        <v>43448</v>
+        <v>31779</v>
       </c>
       <c r="B130" t="inlineStr">
         <is>
-          <t>French Guiana</t>
+          <t>Francia</t>
         </is>
       </c>
       <c r="C130" t="inlineStr">
         <is>
-          <t>French Guiana</t>
-        </is>
-      </c>
-      <c r="E130" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>France</t>
         </is>
       </c>
       <c r="H130" t="inlineStr">
         <is>
-          <t>GF</t>
+          <t>FR</t>
         </is>
       </c>
       <c r="I130" t="inlineStr">
         <is>
-          <t>GUF</t>
+          <t>FRA</t>
         </is>
       </c>
     </row>
@@ -4110,7 +4110,7 @@
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>Guayana Francesa</t>
+          <t>French Guiana</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -4136,26 +4136,31 @@
     </row>
     <row r="132">
       <c r="A132">
-        <v>31769</v>
+        <v>43448</v>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>Guayana Francesa</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Germany</t>
+          <t>French Guiana</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H132" t="inlineStr">
         <is>
-          <t>DE</t>
+          <t>GF</t>
         </is>
       </c>
       <c r="I132" t="inlineStr">
         <is>
-          <t>DEU</t>
+          <t>GUF</t>
         </is>
       </c>
     </row>
@@ -4165,7 +4170,7 @@
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>Alemania</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4186,26 +4191,26 @@
     </row>
     <row r="134">
       <c r="A134">
-        <v>31780</v>
+        <v>31769</v>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Alemania</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Germany</t>
         </is>
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>GR</t>
+          <t>DE</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
         <is>
-          <t>GRC</t>
+          <t>DEU</t>
         </is>
       </c>
     </row>
@@ -4215,7 +4220,7 @@
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>Grecia</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4236,31 +4241,26 @@
     </row>
     <row r="136">
       <c r="A136">
-        <v>31800</v>
+        <v>31780</v>
       </c>
       <c r="B136" t="inlineStr">
         <is>
-          <t>Guadeloupe</t>
+          <t>Grecia</t>
         </is>
       </c>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Guadeloupe</t>
-        </is>
-      </c>
-      <c r="E136" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>GP</t>
+          <t>GR</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
         <is>
-          <t>GLP</t>
+          <t>GRC</t>
         </is>
       </c>
     </row>
@@ -4270,7 +4270,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>Guadalupe</t>
+          <t>Guadeloupe</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4296,51 +4296,56 @@
     </row>
     <row r="138">
       <c r="A138">
-        <v>43449</v>
+        <v>31800</v>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>Guinea Bissau</t>
+          <t>Guadalupe</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Guinea Bissau</t>
+          <t>Guadeloupe</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H138" t="inlineStr">
         <is>
-          <t>GW</t>
+          <t>GP</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
         <is>
-          <t>GNB</t>
+          <t>GLP</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139">
-        <v>43450</v>
+        <v>43449</v>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Guinea Bissau</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Holland</t>
+          <t>Guinea Bissau</t>
         </is>
       </c>
       <c r="H139" t="inlineStr">
         <is>
-          <t>NL</t>
+          <t>GW</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
         <is>
-          <t>NLD</t>
+          <t>GNB</t>
         </is>
       </c>
     </row>
@@ -4350,7 +4355,7 @@
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>Holanda</t>
+          <t>Holland</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
@@ -4371,26 +4376,26 @@
     </row>
     <row r="141">
       <c r="A141">
-        <v>31781</v>
+        <v>43450</v>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Holanda</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
         <is>
-          <t>Hungary</t>
+          <t>Holland</t>
         </is>
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>HU</t>
+          <t>NL</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">
         <is>
-          <t>HUN</t>
+          <t>NLD</t>
         </is>
       </c>
     </row>
@@ -4400,7 +4405,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>Hungría</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
@@ -4421,26 +4426,26 @@
     </row>
     <row r="143">
       <c r="A143">
-        <v>32283</v>
+        <v>31781</v>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Hungría</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
         <is>
-          <t>Iceland</t>
+          <t>Hungary</t>
         </is>
       </c>
       <c r="H143" t="inlineStr">
         <is>
-          <t>IS</t>
+          <t>HU</t>
         </is>
       </c>
       <c r="I143" t="inlineStr">
         <is>
-          <t>ISL</t>
+          <t>HUN</t>
         </is>
       </c>
     </row>
@@ -4450,7 +4455,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>Islandia</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
@@ -4471,76 +4476,76 @@
     </row>
     <row r="145">
       <c r="A145">
-        <v>43451</v>
+        <v>32283</v>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Islandia</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
         <is>
-          <t>India</t>
+          <t>Iceland</t>
         </is>
       </c>
       <c r="H145" t="inlineStr">
         <is>
-          <t>IN</t>
+          <t>IS</t>
         </is>
       </c>
       <c r="I145" t="inlineStr">
         <is>
-          <t>IND</t>
+          <t>ISL</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146">
-        <v>43452</v>
+        <v>43451</v>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
         <is>
-          <t>Indonesia</t>
+          <t>India</t>
         </is>
       </c>
       <c r="H146" t="inlineStr">
         <is>
-          <t>ID</t>
+          <t>IN</t>
         </is>
       </c>
       <c r="I146" t="inlineStr">
         <is>
-          <t>IDN</t>
+          <t>IND</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147">
-        <v>43455</v>
+        <v>43452</v>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Indonesia</t>
         </is>
       </c>
       <c r="H147" t="inlineStr">
         <is>
-          <t>IR</t>
+          <t>ID</t>
         </is>
       </c>
       <c r="I147" t="inlineStr">
         <is>
-          <t>IRN</t>
+          <t>IDN</t>
         </is>
       </c>
     </row>
@@ -4550,7 +4555,7 @@
       </c>
       <c r="B148" t="inlineStr">
         <is>
-          <t>Irán</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="C148" t="inlineStr">
@@ -4571,26 +4576,26 @@
     </row>
     <row r="149">
       <c r="A149">
-        <v>43454</v>
+        <v>43455</v>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Irán</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="H149" t="inlineStr">
         <is>
-          <t>IQ</t>
+          <t>IR</t>
         </is>
       </c>
       <c r="I149" t="inlineStr">
         <is>
-          <t>IRQ</t>
+          <t>IRN</t>
         </is>
       </c>
     </row>
@@ -4600,7 +4605,7 @@
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>Irak</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
@@ -4621,26 +4626,26 @@
     </row>
     <row r="151">
       <c r="A151">
-        <v>31782</v>
+        <v>43454</v>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Irak</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
         <is>
-          <t>Ireland</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="H151" t="inlineStr">
         <is>
-          <t>IE</t>
+          <t>IQ</t>
         </is>
       </c>
       <c r="I151" t="inlineStr">
         <is>
-          <t>IRL</t>
+          <t>IRQ</t>
         </is>
       </c>
     </row>
@@ -4650,7 +4655,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>Irlanda</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4671,51 +4676,51 @@
     </row>
     <row r="153">
       <c r="A153">
-        <v>43456</v>
+        <v>31782</v>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Irlanda</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Ireland</t>
         </is>
       </c>
       <c r="H153" t="inlineStr">
         <is>
-          <t>IL</t>
+          <t>IE</t>
         </is>
       </c>
       <c r="I153" t="inlineStr">
         <is>
-          <t>ISR</t>
+          <t>IRL</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154">
-        <v>31783</v>
+        <v>43456</v>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="H154" t="inlineStr">
         <is>
-          <t>IT</t>
+          <t>IL</t>
         </is>
       </c>
       <c r="I154" t="inlineStr">
         <is>
-          <t>ITA</t>
+          <t>ISR</t>
         </is>
       </c>
     </row>
@@ -4725,7 +4730,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>Italia</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="C155" t="inlineStr">
@@ -4746,26 +4751,26 @@
     </row>
     <row r="156">
       <c r="A156">
-        <v>43457</v>
+        <v>31783</v>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Italia</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Japan</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="H156" t="inlineStr">
         <is>
-          <t>JP</t>
+          <t>IT</t>
         </is>
       </c>
       <c r="I156" t="inlineStr">
         <is>
-          <t>JPN</t>
+          <t>ITA</t>
         </is>
       </c>
     </row>
@@ -4775,7 +4780,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>Japón</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
@@ -4796,26 +4801,26 @@
     </row>
     <row r="158">
       <c r="A158">
-        <v>43458</v>
+        <v>43457</v>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Japón</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Japan</t>
         </is>
       </c>
       <c r="H158" t="inlineStr">
         <is>
-          <t>JO</t>
+          <t>JP</t>
         </is>
       </c>
       <c r="I158" t="inlineStr">
         <is>
-          <t>JOR</t>
+          <t>JPN</t>
         </is>
       </c>
     </row>
@@ -4825,7 +4830,7 @@
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>Jordania</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -4846,16 +4851,26 @@
     </row>
     <row r="160">
       <c r="A160">
-        <v>31811</v>
+        <v>43458</v>
       </c>
       <c r="B160" t="inlineStr">
         <is>
-          <t>Latin America ( 20 Country)</t>
+          <t>Jordania</t>
         </is>
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Latin America ( 20 Country)</t>
+          <t>Jordan</t>
+        </is>
+      </c>
+      <c r="H160" t="inlineStr">
+        <is>
+          <t>JO</t>
+        </is>
+      </c>
+      <c r="I160" t="inlineStr">
+        <is>
+          <t>JOR</t>
         </is>
       </c>
     </row>
@@ -4865,7 +4880,7 @@
       </c>
       <c r="B161" t="inlineStr">
         <is>
-          <t>América Latina (20 países)</t>
+          <t>Latin America ( 20 Country)</t>
         </is>
       </c>
       <c r="C161" t="inlineStr">
@@ -4876,16 +4891,16 @@
     </row>
     <row r="162">
       <c r="A162">
-        <v>31812</v>
+        <v>31811</v>
       </c>
       <c r="B162" t="inlineStr">
         <is>
-          <t>Latin America (19 Country)</t>
+          <t>América Latina (20 países)</t>
         </is>
       </c>
       <c r="C162" t="inlineStr">
         <is>
-          <t>Latin America (19 Country)</t>
+          <t>Latin America ( 20 Country)</t>
         </is>
       </c>
     </row>
@@ -4895,7 +4910,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>América Latina (19 países)</t>
+          <t>Latin America (19 Country)</t>
         </is>
       </c>
       <c r="C163" t="inlineStr">
@@ -4906,16 +4921,16 @@
     </row>
     <row r="164">
       <c r="A164">
-        <v>43053</v>
+        <v>31812</v>
       </c>
       <c r="B164" t="inlineStr">
         <is>
-          <t>Latin America (simple average)</t>
+          <t>América Latina (19 países)</t>
         </is>
       </c>
       <c r="C164" t="inlineStr">
         <is>
-          <t>Latin America (simple average)</t>
+          <t>Latin America (19 Country)</t>
         </is>
       </c>
     </row>
@@ -4925,7 +4940,7 @@
       </c>
       <c r="B165" t="inlineStr">
         <is>
-          <t>América Latina (promedio simple)</t>
+          <t>Latin America (simple average)</t>
         </is>
       </c>
       <c r="C165" t="inlineStr">
@@ -4936,16 +4951,16 @@
     </row>
     <row r="166">
       <c r="A166">
-        <v>43052</v>
+        <v>43053</v>
       </c>
       <c r="B166" t="inlineStr">
         <is>
-          <t>Latin America (weighted average)</t>
+          <t>América Latina (promedio simple)</t>
         </is>
       </c>
       <c r="C166" t="inlineStr">
         <is>
-          <t>Latin America (weighted average)</t>
+          <t>Latin America (simple average)</t>
         </is>
       </c>
     </row>
@@ -4955,7 +4970,7 @@
       </c>
       <c r="B167" t="inlineStr">
         <is>
-          <t>América Latina (promedio ponderado)</t>
+          <t>Latin America (weighted average)</t>
         </is>
       </c>
       <c r="C167" t="inlineStr">
@@ -4966,16 +4981,16 @@
     </row>
     <row r="168">
       <c r="A168">
-        <v>54611</v>
+        <v>43052</v>
       </c>
       <c r="B168" t="inlineStr">
         <is>
-          <t>Latin America and the Caribbean (new serie)</t>
+          <t>América Latina (promedio ponderado)</t>
         </is>
       </c>
       <c r="C168" t="inlineStr">
         <is>
-          <t>Latin America and the Caribbean (new serie)</t>
+          <t>Latin America (weighted average)</t>
         </is>
       </c>
     </row>
@@ -4985,7 +5000,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>América Latina y el Caribe (serie nueva)</t>
+          <t>Latin America and the Caribbean (new serie)</t>
         </is>
       </c>
       <c r="C169" t="inlineStr">
@@ -4996,16 +5011,16 @@
     </row>
     <row r="170">
       <c r="A170">
-        <v>31805</v>
+        <v>54611</v>
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>Latin America except Cuba</t>
+          <t>América Latina y el Caribe (serie nueva)</t>
         </is>
       </c>
       <c r="C170" t="inlineStr">
         <is>
-          <t>Latin America except Cuba</t>
+          <t>Latin America and the Caribbean (new serie)</t>
         </is>
       </c>
     </row>
@@ -5015,7 +5030,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>América Latina excepto Cuba</t>
+          <t>Latin America except Cuba</t>
         </is>
       </c>
       <c r="C171" t="inlineStr">
@@ -5026,16 +5041,16 @@
     </row>
     <row r="172">
       <c r="A172">
-        <v>31806</v>
+        <v>31805</v>
       </c>
       <c r="B172" t="inlineStr">
         <is>
-          <t>Latin American Integration Association (LAIA)</t>
+          <t>América Latina excepto Cuba</t>
         </is>
       </c>
       <c r="C172" t="inlineStr">
         <is>
-          <t>Latin American Integration Association (LAIA)</t>
+          <t>Latin America except Cuba</t>
         </is>
       </c>
     </row>
@@ -5045,7 +5060,7 @@
       </c>
       <c r="B173" t="inlineStr">
         <is>
-          <t>Asociación Latinoamericana de Integración (ALADI)</t>
+          <t>Latin American Integration Association (LAIA)</t>
         </is>
       </c>
       <c r="C173" t="inlineStr">
@@ -5056,26 +5071,16 @@
     </row>
     <row r="174">
       <c r="A174">
-        <v>31784</v>
+        <v>31806</v>
       </c>
       <c r="B174" t="inlineStr">
         <is>
-          <t>Latvia</t>
+          <t>Asociación Latinoamericana de Integración (ALADI)</t>
         </is>
       </c>
       <c r="C174" t="inlineStr">
         <is>
-          <t>Latvia</t>
-        </is>
-      </c>
-      <c r="H174" t="inlineStr">
-        <is>
-          <t>LV</t>
-        </is>
-      </c>
-      <c r="I174" t="inlineStr">
-        <is>
-          <t>LVA</t>
+          <t>Latin American Integration Association (LAIA)</t>
         </is>
       </c>
     </row>
@@ -5085,7 +5090,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Letonia</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="C175" t="inlineStr">
@@ -5106,26 +5111,26 @@
     </row>
     <row r="176">
       <c r="A176">
-        <v>43459</v>
+        <v>31784</v>
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Letonia</t>
         </is>
       </c>
       <c r="C176" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Latvia</t>
         </is>
       </c>
       <c r="H176" t="inlineStr">
         <is>
-          <t>LB</t>
+          <t>LV</t>
         </is>
       </c>
       <c r="I176" t="inlineStr">
         <is>
-          <t>LBN</t>
+          <t>LVA</t>
         </is>
       </c>
     </row>
@@ -5135,7 +5140,7 @@
       </c>
       <c r="B177" t="inlineStr">
         <is>
-          <t>Líbano</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="C177" t="inlineStr">
@@ -5156,26 +5161,26 @@
     </row>
     <row r="178">
       <c r="A178">
-        <v>31785</v>
+        <v>43459</v>
       </c>
       <c r="B178" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Líbano</t>
         </is>
       </c>
       <c r="C178" t="inlineStr">
         <is>
-          <t>Lithuania</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="H178" t="inlineStr">
         <is>
-          <t>LT</t>
+          <t>LB</t>
         </is>
       </c>
       <c r="I178" t="inlineStr">
         <is>
-          <t>LTU</t>
+          <t>LBN</t>
         </is>
       </c>
     </row>
@@ -5185,7 +5190,7 @@
       </c>
       <c r="B179" t="inlineStr">
         <is>
-          <t>Lituania</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="C179" t="inlineStr">
@@ -5206,26 +5211,26 @@
     </row>
     <row r="180">
       <c r="A180">
-        <v>31786</v>
+        <v>31785</v>
       </c>
       <c r="B180" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Lituania</t>
         </is>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Luxembourg</t>
+          <t>Lithuania</t>
         </is>
       </c>
       <c r="H180" t="inlineStr">
         <is>
-          <t>LU</t>
+          <t>LT</t>
         </is>
       </c>
       <c r="I180" t="inlineStr">
         <is>
-          <t>LUX</t>
+          <t>LTU</t>
         </is>
       </c>
     </row>
@@ -5235,7 +5240,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Luxemburgo</t>
+          <t>Luxembourg</t>
         </is>
       </c>
       <c r="C181" t="inlineStr">
@@ -5256,16 +5261,26 @@
     </row>
     <row r="182">
       <c r="A182">
-        <v>31804</v>
+        <v>31786</v>
       </c>
       <c r="B182" t="inlineStr">
         <is>
-          <t>Major International Ristries</t>
+          <t>Luxemburgo</t>
         </is>
       </c>
       <c r="C182" t="inlineStr">
         <is>
-          <t>Major International Ristries</t>
+          <t>Luxembourg</t>
+        </is>
+      </c>
+      <c r="H182" t="inlineStr">
+        <is>
+          <t>LU</t>
+        </is>
+      </c>
+      <c r="I182" t="inlineStr">
+        <is>
+          <t>LUX</t>
         </is>
       </c>
     </row>
@@ -5275,7 +5290,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Principales Registros Internacionales</t>
+          <t>Major International Ristries</t>
         </is>
       </c>
       <c r="C183" t="inlineStr">
@@ -5286,56 +5301,41 @@
     </row>
     <row r="184">
       <c r="A184">
-        <v>31787</v>
+        <v>31804</v>
       </c>
       <c r="B184" t="inlineStr">
         <is>
-          <t>Malta</t>
+          <t>Principales Registros Internacionales</t>
         </is>
       </c>
       <c r="C184" t="inlineStr">
         <is>
-          <t>Malta</t>
-        </is>
-      </c>
-      <c r="H184" t="inlineStr">
-        <is>
-          <t>MT</t>
-        </is>
-      </c>
-      <c r="I184" t="inlineStr">
-        <is>
-          <t>MLT</t>
+          <t>Major International Ristries</t>
         </is>
       </c>
     </row>
     <row r="185">
       <c r="A185">
-        <v>43406</v>
+        <v>31787</v>
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>Martinique</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="C185" t="inlineStr">
         <is>
-          <t>Martinique</t>
-        </is>
-      </c>
-      <c r="E185" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Malta</t>
         </is>
       </c>
       <c r="H185" t="inlineStr">
         <is>
-          <t>MQ</t>
+          <t>MT</t>
         </is>
       </c>
       <c r="I185" t="inlineStr">
         <is>
-          <t>MTQ</t>
+          <t>MLT</t>
         </is>
       </c>
     </row>
@@ -5345,7 +5345,7 @@
       </c>
       <c r="B186" t="inlineStr">
         <is>
-          <t>Martinica</t>
+          <t>Martinique</t>
         </is>
       </c>
       <c r="C186" t="inlineStr">
@@ -5371,16 +5371,16 @@
     </row>
     <row r="187">
       <c r="A187">
-        <v>236</v>
+        <v>43406</v>
       </c>
       <c r="B187" t="inlineStr">
         <is>
-          <t>Montserrat</t>
+          <t>Martinica</t>
         </is>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Montserrat</t>
+          <t>Martinique</t>
         </is>
       </c>
       <c r="E187" t="inlineStr">
@@ -5390,37 +5390,42 @@
       </c>
       <c r="H187" t="inlineStr">
         <is>
-          <t>MS</t>
+          <t>MQ</t>
         </is>
       </c>
       <c r="I187" t="inlineStr">
         <is>
-          <t>MSR</t>
+          <t>MTQ</t>
         </is>
       </c>
     </row>
     <row r="188">
       <c r="A188">
-        <v>43460</v>
+        <v>236</v>
       </c>
       <c r="B188" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Montserrat</t>
         </is>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Morocco</t>
+          <t>Montserrat</t>
+        </is>
+      </c>
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H188" t="inlineStr">
         <is>
-          <t>MA</t>
+          <t>MS</t>
         </is>
       </c>
       <c r="I188" t="inlineStr">
         <is>
-          <t>MAR</t>
+          <t>MSR</t>
         </is>
       </c>
     </row>
@@ -5430,7 +5435,7 @@
       </c>
       <c r="B189" t="inlineStr">
         <is>
-          <t>Marruecos</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="C189" t="inlineStr">
@@ -5451,41 +5456,51 @@
     </row>
     <row r="190">
       <c r="A190">
-        <v>43461</v>
+        <v>43460</v>
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Marruecos</t>
         </is>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Mozambique</t>
+          <t>Morocco</t>
         </is>
       </c>
       <c r="H190" t="inlineStr">
         <is>
-          <t>MZ</t>
+          <t>MA</t>
         </is>
       </c>
       <c r="I190" t="inlineStr">
         <is>
-          <t>MOZ</t>
+          <t>MAR</t>
         </is>
       </c>
     </row>
     <row r="191">
       <c r="A191">
-        <v>31788</v>
+        <v>43461</v>
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Mozambique</t>
         </is>
       </c>
       <c r="C191" t="inlineStr">
         <is>
-          <t>Netherlands</t>
+          <t>Mozambique</t>
+        </is>
+      </c>
+      <c r="H191" t="inlineStr">
+        <is>
+          <t>MZ</t>
+        </is>
+      </c>
+      <c r="I191" t="inlineStr">
+        <is>
+          <t>MOZ</t>
         </is>
       </c>
     </row>
@@ -5495,7 +5510,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>Países Bajos</t>
+          <t>Netherlands</t>
         </is>
       </c>
       <c r="C192" t="inlineStr">
@@ -5506,16 +5521,16 @@
     </row>
     <row r="193">
       <c r="A193">
-        <v>215</v>
+        <v>31788</v>
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>Netherlands Antilles</t>
+          <t>Países Bajos</t>
         </is>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Netherlands Antilles</t>
+          <t>Netherlands</t>
         </is>
       </c>
     </row>
@@ -5525,7 +5540,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>Ex Antillas Neerlandesas</t>
+          <t>Netherlands Antilles</t>
         </is>
       </c>
       <c r="C194" t="inlineStr">
@@ -5536,51 +5551,41 @@
     </row>
     <row r="195">
       <c r="A195">
-        <v>43462</v>
+        <v>215</v>
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>Nigeria</t>
+          <t>Ex Antillas Neerlandesas</t>
         </is>
       </c>
       <c r="C195" t="inlineStr">
         <is>
-          <t>Nigeria</t>
-        </is>
-      </c>
-      <c r="H195" t="inlineStr">
-        <is>
-          <t>NG</t>
-        </is>
-      </c>
-      <c r="I195" t="inlineStr">
-        <is>
-          <t>NGA</t>
+          <t>Netherlands Antilles</t>
         </is>
       </c>
     </row>
     <row r="196">
       <c r="A196">
-        <v>32284</v>
+        <v>43462</v>
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="C196" t="inlineStr">
         <is>
-          <t>Norway</t>
+          <t>Nigeria</t>
         </is>
       </c>
       <c r="H196" t="inlineStr">
         <is>
-          <t>NO</t>
+          <t>NG</t>
         </is>
       </c>
       <c r="I196" t="inlineStr">
         <is>
-          <t>NOR</t>
+          <t>NGA</t>
         </is>
       </c>
     </row>
@@ -5590,7 +5595,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>Noruega</t>
+          <t>Norway</t>
         </is>
       </c>
       <c r="C197" t="inlineStr">
@@ -5611,16 +5616,26 @@
     </row>
     <row r="198">
       <c r="A198">
-        <v>77271</v>
+        <v>32284</v>
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>OECD Organization for Economic Cooperation and Development</t>
+          <t>Noruega</t>
         </is>
       </c>
       <c r="C198" t="inlineStr">
         <is>
-          <t>OECD Organization for Economic Cooperation and Development</t>
+          <t>Norway</t>
+        </is>
+      </c>
+      <c r="H198" t="inlineStr">
+        <is>
+          <t>NO</t>
+        </is>
+      </c>
+      <c r="I198" t="inlineStr">
+        <is>
+          <t>NOR</t>
         </is>
       </c>
     </row>
@@ -5630,7 +5645,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>OCDE Organización para la Cooperación y Desarrollo Económico</t>
+          <t>OECD Organization for Economic Cooperation and Development</t>
         </is>
       </c>
       <c r="C199" t="inlineStr">
@@ -5641,16 +5656,16 @@
     </row>
     <row r="200">
       <c r="A200">
-        <v>31802</v>
+        <v>77271</v>
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>Other East Coast of South America</t>
+          <t>OCDE Organización para la Cooperación y Desarrollo Económico</t>
         </is>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Other East Coast of South America</t>
+          <t>OECD Organization for Economic Cooperation and Development</t>
         </is>
       </c>
     </row>
@@ -5660,7 +5675,7 @@
       </c>
       <c r="B201" t="inlineStr">
         <is>
-          <t>Otros países costa este América del Sur</t>
+          <t>Other East Coast of South America</t>
         </is>
       </c>
       <c r="C201" t="inlineStr">
@@ -5671,16 +5686,16 @@
     </row>
     <row r="202">
       <c r="A202">
-        <v>31803</v>
+        <v>31802</v>
       </c>
       <c r="B202" t="inlineStr">
         <is>
-          <t>Other West Coast of South America</t>
+          <t>Otros países costa este América del Sur</t>
         </is>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Other West Coast of South America</t>
+          <t>Other East Coast of South America</t>
         </is>
       </c>
     </row>
@@ -5690,7 +5705,7 @@
       </c>
       <c r="B203" t="inlineStr">
         <is>
-          <t>Otros países costa oeste América del Sur</t>
+          <t>Other West Coast of South America</t>
         </is>
       </c>
       <c r="C203" t="inlineStr">
@@ -5701,16 +5716,16 @@
     </row>
     <row r="204">
       <c r="A204">
-        <v>46576</v>
+        <v>31803</v>
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>Other countries</t>
+          <t>Otros países costa oeste América del Sur</t>
         </is>
       </c>
       <c r="C204" t="inlineStr">
         <is>
-          <t>Other countries</t>
+          <t>Other West Coast of South America</t>
         </is>
       </c>
     </row>
@@ -5720,7 +5735,7 @@
       </c>
       <c r="B205" t="inlineStr">
         <is>
-          <t>Otros países</t>
+          <t>Other countries</t>
         </is>
       </c>
       <c r="C205" t="inlineStr">
@@ -5731,26 +5746,16 @@
     </row>
     <row r="206">
       <c r="A206">
-        <v>43472</v>
+        <v>46576</v>
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>Philippines</t>
+          <t>Otros países</t>
         </is>
       </c>
       <c r="C206" t="inlineStr">
         <is>
-          <t>Philippines</t>
-        </is>
-      </c>
-      <c r="H206" t="inlineStr">
-        <is>
-          <t>PH</t>
-        </is>
-      </c>
-      <c r="I206" t="inlineStr">
-        <is>
-          <t>PHL</t>
+          <t>Other countries</t>
         </is>
       </c>
     </row>
@@ -5760,7 +5765,7 @@
       </c>
       <c r="B207" t="inlineStr">
         <is>
-          <t>Filipinas</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="C207" t="inlineStr">
@@ -5781,26 +5786,26 @@
     </row>
     <row r="208">
       <c r="A208">
-        <v>31789</v>
+        <v>43472</v>
       </c>
       <c r="B208" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Filipinas</t>
         </is>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Poland</t>
+          <t>Philippines</t>
         </is>
       </c>
       <c r="H208" t="inlineStr">
         <is>
-          <t>PL</t>
+          <t>PH</t>
         </is>
       </c>
       <c r="I208" t="inlineStr">
         <is>
-          <t>POL</t>
+          <t>PHL</t>
         </is>
       </c>
     </row>
@@ -5810,7 +5815,7 @@
       </c>
       <c r="B209" t="inlineStr">
         <is>
-          <t>Polonia</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="C209" t="inlineStr">
@@ -5831,81 +5836,81 @@
     </row>
     <row r="210">
       <c r="A210">
-        <v>20377</v>
+        <v>31789</v>
       </c>
       <c r="B210" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Polonia</t>
         </is>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Portugal</t>
+          <t>Poland</t>
         </is>
       </c>
       <c r="H210" t="inlineStr">
         <is>
-          <t>PT</t>
+          <t>PL</t>
         </is>
       </c>
       <c r="I210" t="inlineStr">
         <is>
-          <t>PRT</t>
+          <t>POL</t>
         </is>
       </c>
     </row>
     <row r="211">
       <c r="A211">
-        <v>261</v>
+        <v>20377</v>
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="C211" t="inlineStr">
         <is>
-          <t>Puerto Rico</t>
-        </is>
-      </c>
-      <c r="E211" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Portugal</t>
         </is>
       </c>
       <c r="H211" t="inlineStr">
         <is>
-          <t>PR</t>
+          <t>PT</t>
         </is>
       </c>
       <c r="I211" t="inlineStr">
         <is>
-          <t>PRI</t>
+          <t>PRT</t>
         </is>
       </c>
     </row>
     <row r="212">
       <c r="A212">
-        <v>43471</v>
+        <v>261</v>
       </c>
       <c r="B212" t="inlineStr">
         <is>
-          <t>Republic of Korea (South Korea)</t>
+          <t>Puerto Rico</t>
         </is>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Republic of Korea (South Korea)</t>
+          <t>Puerto Rico</t>
+        </is>
+      </c>
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H212" t="inlineStr">
         <is>
-          <t>KR</t>
+          <t>PR</t>
         </is>
       </c>
       <c r="I212" t="inlineStr">
         <is>
-          <t>KOR</t>
+          <t>PRI</t>
         </is>
       </c>
     </row>
@@ -5915,7 +5920,7 @@
       </c>
       <c r="B213" t="inlineStr">
         <is>
-          <t>República de Corea (Corea del Sur)</t>
+          <t>Republic of Korea (South Korea)</t>
         </is>
       </c>
       <c r="C213" t="inlineStr">
@@ -5936,26 +5941,26 @@
     </row>
     <row r="214">
       <c r="A214">
-        <v>31792</v>
+        <v>43471</v>
       </c>
       <c r="B214" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>República de Corea (Corea del Sur)</t>
         </is>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Romania</t>
+          <t>Republic of Korea (South Korea)</t>
         </is>
       </c>
       <c r="H214" t="inlineStr">
         <is>
-          <t>RO</t>
+          <t>KR</t>
         </is>
       </c>
       <c r="I214" t="inlineStr">
         <is>
-          <t>ROU</t>
+          <t>KOR</t>
         </is>
       </c>
     </row>
@@ -5965,7 +5970,7 @@
       </c>
       <c r="B215" t="inlineStr">
         <is>
-          <t>Rumania</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="C215" t="inlineStr">
@@ -5986,26 +5991,26 @@
     </row>
     <row r="216">
       <c r="A216">
-        <v>43464</v>
+        <v>31792</v>
       </c>
       <c r="B216" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Rumania</t>
         </is>
       </c>
       <c r="C216" t="inlineStr">
         <is>
-          <t>Russia</t>
+          <t>Romania</t>
         </is>
       </c>
       <c r="H216" t="inlineStr">
         <is>
-          <t>RU</t>
+          <t>RO</t>
         </is>
       </c>
       <c r="I216" t="inlineStr">
         <is>
-          <t>RUS</t>
+          <t>ROU</t>
         </is>
       </c>
     </row>
@@ -6015,7 +6020,7 @@
       </c>
       <c r="B217" t="inlineStr">
         <is>
-          <t>Rusia</t>
+          <t>Russia</t>
         </is>
       </c>
       <c r="C217" t="inlineStr">
@@ -6036,31 +6041,41 @@
     </row>
     <row r="218">
       <c r="A218">
-        <v>85582</v>
+        <v>43464</v>
       </c>
       <c r="B218" t="inlineStr">
         <is>
-          <t>SICA</t>
+          <t>Rusia</t>
         </is>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>SICA</t>
+          <t>Russia</t>
+        </is>
+      </c>
+      <c r="H218" t="inlineStr">
+        <is>
+          <t>RU</t>
+        </is>
+      </c>
+      <c r="I218" t="inlineStr">
+        <is>
+          <t>RUS</t>
         </is>
       </c>
     </row>
     <row r="219">
       <c r="A219">
-        <v>43445</v>
+        <v>85582</v>
       </c>
       <c r="B219" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>SICA</t>
         </is>
       </c>
       <c r="C219" t="inlineStr">
         <is>
-          <t>Scotland</t>
+          <t>SICA</t>
         </is>
       </c>
     </row>
@@ -6070,7 +6085,7 @@
       </c>
       <c r="B220" t="inlineStr">
         <is>
-          <t>Escocia</t>
+          <t>Scotland</t>
         </is>
       </c>
       <c r="C220" t="inlineStr">
@@ -6081,31 +6096,16 @@
     </row>
     <row r="221">
       <c r="A221">
-        <v>43405</v>
+        <v>43445</v>
       </c>
       <c r="B221" t="inlineStr">
         <is>
-          <t>Sint Maarten (Dutch part)</t>
+          <t>Escocia</t>
         </is>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Sint Maarten (Dutch part)</t>
-        </is>
-      </c>
-      <c r="E221" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="H221" t="inlineStr">
-        <is>
-          <t>SX</t>
-        </is>
-      </c>
-      <c r="I221" t="inlineStr">
-        <is>
-          <t>SXM</t>
+          <t>Scotland</t>
         </is>
       </c>
     </row>
@@ -6115,7 +6115,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>San Martín (parte de los Países Bajos)</t>
+          <t>Sint Maarten (Dutch part)</t>
         </is>
       </c>
       <c r="C222" t="inlineStr">
@@ -6141,799 +6141,859 @@
     </row>
     <row r="223">
       <c r="A223">
-        <v>31775</v>
+        <v>43405</v>
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>San Martín (parte de los Países Bajos)</t>
         </is>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Sint Maarten (Dutch part)</t>
+        </is>
+      </c>
+      <c r="E223" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H223" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>SX</t>
         </is>
       </c>
       <c r="I223" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>SXM</t>
         </is>
       </c>
     </row>
     <row r="224">
       <c r="A224">
-        <v>31775</v>
+        <v>43405</v>
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Eslovaquia</t>
+          <t>Sint Maarten</t>
         </is>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Slovakia</t>
+          <t>Sint Maarten (Dutch part)</t>
+        </is>
+      </c>
+      <c r="E224" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H224" t="inlineStr">
         <is>
-          <t>SK</t>
+          <t>SX</t>
         </is>
       </c>
       <c r="I224" t="inlineStr">
         <is>
-          <t>SVK</t>
+          <t>SXM</t>
         </is>
       </c>
     </row>
     <row r="225">
       <c r="A225">
-        <v>31776</v>
+        <v>31775</v>
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="H225" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="I225" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>SVK</t>
         </is>
       </c>
     </row>
     <row r="226">
       <c r="A226">
-        <v>31776</v>
+        <v>31775</v>
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Eslovenia</t>
+          <t>Eslovaquia</t>
         </is>
       </c>
       <c r="C226" t="inlineStr">
         <is>
-          <t>Slovenia</t>
+          <t>Slovakia</t>
         </is>
       </c>
       <c r="H226" t="inlineStr">
         <is>
-          <t>SI</t>
+          <t>SK</t>
         </is>
       </c>
       <c r="I226" t="inlineStr">
         <is>
-          <t>SVN</t>
+          <t>SVK</t>
         </is>
       </c>
     </row>
     <row r="227">
       <c r="A227">
-        <v>43466</v>
+        <v>31776</v>
       </c>
       <c r="B227" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="C227" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="H227" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="I227" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>SVN</t>
         </is>
       </c>
     </row>
     <row r="228">
       <c r="A228">
-        <v>43466</v>
+        <v>31776</v>
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>Sudáfrica</t>
+          <t>Eslovenia</t>
         </is>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>South Africa</t>
+          <t>Slovenia</t>
         </is>
       </c>
       <c r="H228" t="inlineStr">
         <is>
-          <t>ZA</t>
+          <t>SI</t>
         </is>
       </c>
       <c r="I228" t="inlineStr">
         <is>
-          <t>ZAF</t>
+          <t>SVN</t>
         </is>
       </c>
     </row>
     <row r="229">
       <c r="A229">
-        <v>20378</v>
+        <v>43466</v>
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="C229" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="H229" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="I229" t="inlineStr">
         <is>
-          <t>ESP</t>
+          <t>ZAF</t>
         </is>
       </c>
     </row>
     <row r="230">
       <c r="A230">
-        <v>20378</v>
+        <v>43466</v>
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>España</t>
+          <t>Sudáfrica</t>
         </is>
       </c>
       <c r="C230" t="inlineStr">
         <is>
-          <t>Spain</t>
+          <t>South Africa</t>
         </is>
       </c>
       <c r="H230" t="inlineStr">
         <is>
-          <t>ES</t>
+          <t>ZA</t>
         </is>
       </c>
       <c r="I230" t="inlineStr">
         <is>
-          <t>ESP</t>
+          <t>ZAF</t>
         </is>
       </c>
     </row>
     <row r="231">
       <c r="A231">
-        <v>31793</v>
+        <v>20378</v>
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="C231" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H231" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="I231" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>ESP</t>
         </is>
       </c>
     </row>
     <row r="232">
       <c r="A232">
-        <v>31793</v>
+        <v>20378</v>
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>Suecia</t>
+          <t>España</t>
         </is>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Sweden</t>
+          <t>Spain</t>
         </is>
       </c>
       <c r="H232" t="inlineStr">
         <is>
-          <t>SE</t>
+          <t>ES</t>
         </is>
       </c>
       <c r="I232" t="inlineStr">
         <is>
-          <t>SWE</t>
+          <t>ESP</t>
         </is>
       </c>
     </row>
     <row r="233">
       <c r="A233">
-        <v>32285</v>
+        <v>31793</v>
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="C233" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="H233" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="I233" t="inlineStr">
         <is>
-          <t>CHE</t>
+          <t>SWE</t>
         </is>
       </c>
     </row>
     <row r="234">
       <c r="A234">
-        <v>32285</v>
+        <v>31793</v>
       </c>
       <c r="B234" t="inlineStr">
         <is>
-          <t>Suiza</t>
+          <t>Suecia</t>
         </is>
       </c>
       <c r="C234" t="inlineStr">
         <is>
-          <t>Switzerland</t>
+          <t>Sweden</t>
         </is>
       </c>
       <c r="H234" t="inlineStr">
         <is>
-          <t>CH</t>
+          <t>SE</t>
         </is>
       </c>
       <c r="I234" t="inlineStr">
         <is>
-          <t>CHE</t>
+          <t>SWE</t>
         </is>
       </c>
     </row>
     <row r="235">
       <c r="A235">
-        <v>43465</v>
+        <v>32285</v>
       </c>
       <c r="B235" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="C235" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="H235" t="inlineStr">
         <is>
-          <t>SY</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="I235" t="inlineStr">
         <is>
-          <t>SYR</t>
+          <t>CHE</t>
         </is>
       </c>
     </row>
     <row r="236">
       <c r="A236">
-        <v>43465</v>
+        <v>32285</v>
       </c>
       <c r="B236" t="inlineStr">
         <is>
-          <t>Siria</t>
+          <t>Suiza</t>
         </is>
       </c>
       <c r="C236" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Switzerland</t>
         </is>
       </c>
       <c r="H236" t="inlineStr">
         <is>
-          <t>SY</t>
+          <t>CH</t>
         </is>
       </c>
       <c r="I236" t="inlineStr">
         <is>
-          <t>SYR</t>
+          <t>CHE</t>
         </is>
       </c>
     </row>
     <row r="237">
       <c r="A237">
-        <v>43469</v>
+        <v>43465</v>
       </c>
       <c r="B237" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="C237" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="H237" t="inlineStr">
         <is>
-          <t>TW</t>
+          <t>SY</t>
         </is>
       </c>
       <c r="I237" t="inlineStr">
         <is>
-          <t>TWN</t>
+          <t>SYR</t>
         </is>
       </c>
     </row>
     <row r="238">
       <c r="A238">
-        <v>43469</v>
+        <v>43465</v>
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>Taiwán</t>
+          <t>Siria</t>
         </is>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Taiwan</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="H238" t="inlineStr">
         <is>
-          <t>TW</t>
+          <t>SY</t>
         </is>
       </c>
       <c r="I238" t="inlineStr">
         <is>
-          <t>TWN</t>
+          <t>SYR</t>
         </is>
       </c>
     </row>
     <row r="239">
       <c r="A239">
-        <v>31810</v>
+        <v>43469</v>
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>The Caribbean Community (CARICOM)</t>
+          <t>Taiwan</t>
         </is>
       </c>
       <c r="C239" t="inlineStr">
         <is>
-          <t>The Caribbean Community (CARICOM)</t>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="H239" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="I239" t="inlineStr">
+        <is>
+          <t>TWN</t>
         </is>
       </c>
     </row>
     <row r="240">
       <c r="A240">
-        <v>31810</v>
+        <v>43469</v>
       </c>
       <c r="B240" t="inlineStr">
         <is>
-          <t>Comunidad del Caribe (CARICOM)</t>
+          <t>Taiwán</t>
         </is>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>The Caribbean Community (CARICOM)</t>
+          <t>Taiwan</t>
+        </is>
+      </c>
+      <c r="H240" t="inlineStr">
+        <is>
+          <t>TW</t>
+        </is>
+      </c>
+      <c r="I240" t="inlineStr">
+        <is>
+          <t>TWN</t>
         </is>
       </c>
     </row>
     <row r="241">
       <c r="A241">
-        <v>43530</v>
+        <v>31810</v>
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>The Caribbean Community (CARICOM)</t>
         </is>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="H241" t="inlineStr">
-        <is>
-          <t>TR</t>
-        </is>
-      </c>
-      <c r="I241" t="inlineStr">
-        <is>
-          <t>TUR</t>
+          <t>The Caribbean Community (CARICOM)</t>
         </is>
       </c>
     </row>
     <row r="242">
       <c r="A242">
-        <v>43530</v>
+        <v>31810</v>
       </c>
       <c r="B242" t="inlineStr">
         <is>
-          <t>Turquía</t>
+          <t>Comunidad del Caribe (CARICOM)</t>
         </is>
       </c>
       <c r="C242" t="inlineStr">
         <is>
-          <t>Turkey</t>
-        </is>
-      </c>
-      <c r="H242" t="inlineStr">
-        <is>
-          <t>TR</t>
-        </is>
-      </c>
-      <c r="I242" t="inlineStr">
-        <is>
-          <t>TUR</t>
+          <t>The Caribbean Community (CARICOM)</t>
         </is>
       </c>
     </row>
     <row r="243">
       <c r="A243">
-        <v>3272</v>
+        <v>43530</v>
       </c>
       <c r="B243" t="inlineStr">
         <is>
-          <t>Turks and Caicos Islands</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="C243" t="inlineStr">
         <is>
-          <t>Turks and Caicos Islands</t>
-        </is>
-      </c>
-      <c r="E243" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="H243" t="inlineStr">
         <is>
-          <t>TC</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="I243" t="inlineStr">
         <is>
-          <t>TCA</t>
+          <t>TUR</t>
         </is>
       </c>
     </row>
     <row r="244">
       <c r="A244">
-        <v>3272</v>
+        <v>43530</v>
       </c>
       <c r="B244" t="inlineStr">
         <is>
-          <t>Islas Turcas y Caicos</t>
+          <t>Turquía</t>
         </is>
       </c>
       <c r="C244" t="inlineStr">
         <is>
-          <t>Turks and Caicos Islands</t>
-        </is>
-      </c>
-      <c r="E244" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="H244" t="inlineStr">
         <is>
-          <t>TC</t>
+          <t>TR</t>
         </is>
       </c>
       <c r="I244" t="inlineStr">
         <is>
-          <t>TCA</t>
+          <t>TUR</t>
         </is>
       </c>
     </row>
     <row r="245">
       <c r="A245">
-        <v>43467</v>
+        <v>3272</v>
       </c>
       <c r="B245" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Turks and Caicos Islands</t>
         </is>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Turks and Caicos Islands</t>
+        </is>
+      </c>
+      <c r="E245" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H245" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>TC</t>
         </is>
       </c>
       <c r="I245" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TCA</t>
         </is>
       </c>
     </row>
     <row r="246">
       <c r="A246">
-        <v>43467</v>
+        <v>3272</v>
       </c>
       <c r="B246" t="inlineStr">
         <is>
-          <t>Ucrania</t>
+          <t>Islas Turcas y Caicos</t>
         </is>
       </c>
       <c r="C246" t="inlineStr">
         <is>
-          <t>Ukraine</t>
+          <t>Turks and Caicos Islands</t>
+        </is>
+      </c>
+      <c r="E246" t="inlineStr">
+        <is>
+          <t>Y</t>
         </is>
       </c>
       <c r="H246" t="inlineStr">
         <is>
-          <t>UA</t>
+          <t>TC</t>
         </is>
       </c>
       <c r="I246" t="inlineStr">
         <is>
-          <t>UKR</t>
+          <t>TCA</t>
         </is>
       </c>
     </row>
     <row r="247">
       <c r="A247">
-        <v>31790</v>
+        <v>43467</v>
       </c>
       <c r="B247" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="H247" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="I247" t="inlineStr">
         <is>
-          <t>GBR</t>
+          <t>UKR</t>
         </is>
       </c>
     </row>
     <row r="248">
       <c r="A248">
-        <v>31790</v>
+        <v>43467</v>
       </c>
       <c r="B248" t="inlineStr">
         <is>
-          <t>Reino Unido</t>
+          <t>Ucrania</t>
         </is>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Ukraine</t>
         </is>
       </c>
       <c r="H248" t="inlineStr">
         <is>
-          <t>GB</t>
+          <t>UA</t>
         </is>
       </c>
       <c r="I248" t="inlineStr">
         <is>
-          <t>GBR</t>
+          <t>UKR</t>
         </is>
       </c>
     </row>
     <row r="249">
       <c r="A249">
-        <v>43446</v>
+        <v>31790</v>
       </c>
       <c r="B249" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="H249" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="I249" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>GBR</t>
         </is>
       </c>
     </row>
     <row r="250">
       <c r="A250">
-        <v>43446</v>
+        <v>31790</v>
       </c>
       <c r="B250" t="inlineStr">
         <is>
-          <t>Estados Unidos</t>
+          <t>Reino Unido</t>
         </is>
       </c>
       <c r="C250" t="inlineStr">
         <is>
-          <t>United States</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="H250" t="inlineStr">
         <is>
-          <t>US</t>
+          <t>GB</t>
         </is>
       </c>
       <c r="I250" t="inlineStr">
         <is>
-          <t>USA</t>
+          <t>GBR</t>
         </is>
       </c>
     </row>
     <row r="251">
       <c r="A251">
-        <v>245</v>
+        <v>43446</v>
       </c>
       <c r="B251" t="inlineStr">
         <is>
-          <t>United States Virgin Islands</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>United States Virgin Islands</t>
-        </is>
-      </c>
-      <c r="E251" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H251" t="inlineStr">
         <is>
-          <t>VI</t>
+          <t>US</t>
         </is>
       </c>
       <c r="I251" t="inlineStr">
         <is>
-          <t>VIR</t>
+          <t>USA</t>
         </is>
       </c>
     </row>
     <row r="252">
       <c r="A252">
-        <v>245</v>
+        <v>43446</v>
       </c>
       <c r="B252" t="inlineStr">
         <is>
-          <t>Islas Vírgenes de los Estados Unidos</t>
+          <t>Estados Unidos</t>
         </is>
       </c>
       <c r="C252" t="inlineStr">
         <is>
-          <t>United States Virgin Islands</t>
-        </is>
-      </c>
-      <c r="E252" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>United States</t>
         </is>
       </c>
       <c r="H252" t="inlineStr">
         <is>
-          <t>VI</t>
+          <t>US</t>
         </is>
       </c>
       <c r="I252" t="inlineStr">
         <is>
-          <t>VIR</t>
+          <t>USA</t>
         </is>
       </c>
     </row>
     <row r="253">
       <c r="A253">
-        <v>47707</v>
+        <v>245</v>
       </c>
       <c r="B253" t="inlineStr">
         <is>
-          <t>World</t>
+          <t>United States Virgin Islands</t>
         </is>
       </c>
       <c r="C253" t="inlineStr">
         <is>
-          <t>World</t>
-        </is>
-      </c>
-      <c r="G253" t="inlineStr">
-        <is>
-          <t>Y</t>
+          <t>United States Virgin Islands</t>
+        </is>
+      </c>
+      <c r="E253" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H253" t="inlineStr">
+        <is>
+          <t>VI</t>
         </is>
       </c>
       <c r="I253" t="inlineStr">
         <is>
-          <t>WLD</t>
+          <t>VIR</t>
         </is>
       </c>
     </row>
     <row r="254">
       <c r="A254">
+        <v>245</v>
+      </c>
+      <c r="B254" t="inlineStr">
+        <is>
+          <t>Islas Vírgenes de los Estados Unidos</t>
+        </is>
+      </c>
+      <c r="C254" t="inlineStr">
+        <is>
+          <t>United States Virgin Islands</t>
+        </is>
+      </c>
+      <c r="E254" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="H254" t="inlineStr">
+        <is>
+          <t>VI</t>
+        </is>
+      </c>
+      <c r="I254" t="inlineStr">
+        <is>
+          <t>VIR</t>
+        </is>
+      </c>
+    </row>
+    <row r="255">
+      <c r="A255">
         <v>47707</v>
       </c>
-      <c r="B254" t="inlineStr">
+      <c r="B255" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="C255" t="inlineStr">
+        <is>
+          <t>World</t>
+        </is>
+      </c>
+      <c r="G255" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="I255" t="inlineStr">
+        <is>
+          <t>WLD</t>
+        </is>
+      </c>
+    </row>
+    <row r="256">
+      <c r="A256">
+        <v>47707</v>
+      </c>
+      <c r="B256" t="inlineStr">
         <is>
           <t>Mundo</t>
         </is>
       </c>
-      <c r="C254" t="inlineStr">
+      <c r="C256" t="inlineStr">
         <is>
           <t>World</t>
         </is>
       </c>
-      <c r="G254" t="inlineStr">
-        <is>
-          <t>Y</t>
-        </is>
-      </c>
-      <c r="I254" t="inlineStr">
+      <c r="G256" t="inlineStr">
+        <is>
+          <t>Y</t>
+        </is>
+      </c>
+      <c r="I256" t="inlineStr">
         <is>
           <t>WLD</t>
         </is>

</xml_diff>